<commit_message>
updated certifications Escel sheet
</commit_message>
<xml_diff>
--- a/comprehensive_grocery_certifications.xlsx
+++ b/comprehensive_grocery_certifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StardogChampion\tbl-grocery-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD085BD-210F-40A5-9E7C-775FE19D7CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA922984-178C-475E-B331-33C7F2C512BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="888">
   <si>
     <t>Product_Brand</t>
   </si>
@@ -2679,6 +2679,12 @@
   </si>
   <si>
     <t>Generated: 2026-01-13 21:08:12</t>
+  </si>
+  <si>
+    <t>Ben &amp; Jerry's</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -3067,11 +3073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J893"/>
+  <dimension ref="A1:J894"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A866" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A866" sqref="A866"/>
+      <pane ySplit="1" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J652" sqref="J652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21322,17 +21328,17 @@
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A652" s="2" t="s">
-        <v>47</v>
+        <v>886</v>
       </c>
       <c r="B652" s="2" t="s">
         <v>653</v>
       </c>
       <c r="C652" s="2"/>
       <c r="D652" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E652" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F652" s="3" t="b">
         <v>0</v>
@@ -21341,16 +21347,16 @@
         <v>0</v>
       </c>
       <c r="H652" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I652" s="2"/>
       <c r="J652" s="2" t="s">
-        <v>12</v>
+        <v>887</v>
       </c>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A653" s="2" t="s">
-        <v>656</v>
+        <v>47</v>
       </c>
       <c r="B653" s="2" t="s">
         <v>653</v>
@@ -21378,7 +21384,7 @@
     </row>
     <row r="654" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B654" s="2" t="s">
         <v>653</v>
@@ -21406,7 +21412,7 @@
     </row>
     <row r="655" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A655" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B655" s="2" t="s">
         <v>653</v>
@@ -21434,7 +21440,7 @@
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A656" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B656" s="2" t="s">
         <v>653</v>
@@ -21462,7 +21468,7 @@
     </row>
     <row r="657" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A657" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B657" s="2" t="s">
         <v>653</v>
@@ -21490,7 +21496,7 @@
     </row>
     <row r="658" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A658" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B658" s="2" t="s">
         <v>653</v>
@@ -21518,7 +21524,7 @@
     </row>
     <row r="659" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A659" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B659" s="2" t="s">
         <v>653</v>
@@ -21546,7 +21552,7 @@
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A660" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B660" s="2" t="s">
         <v>653</v>
@@ -21574,7 +21580,7 @@
     </row>
     <row r="661" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A661" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B661" s="2" t="s">
         <v>653</v>
@@ -21602,7 +21608,7 @@
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A662" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B662" s="2" t="s">
         <v>653</v>
@@ -21630,7 +21636,7 @@
     </row>
     <row r="663" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B663" s="2" t="s">
         <v>653</v>
@@ -21658,7 +21664,7 @@
     </row>
     <row r="664" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A664" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B664" s="2" t="s">
         <v>653</v>
@@ -21686,7 +21692,7 @@
     </row>
     <row r="665" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A665" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B665" s="2" t="s">
         <v>653</v>
@@ -21714,7 +21720,7 @@
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A666" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B666" s="2" t="s">
         <v>653</v>
@@ -21742,7 +21748,7 @@
     </row>
     <row r="667" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A667" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B667" s="2" t="s">
         <v>653</v>
@@ -21770,7 +21776,7 @@
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A668" s="2" t="s">
-        <v>333</v>
+        <v>670</v>
       </c>
       <c r="B668" s="2" t="s">
         <v>653</v>
@@ -21798,7 +21804,7 @@
     </row>
     <row r="669" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A669" s="2" t="s">
-        <v>671</v>
+        <v>333</v>
       </c>
       <c r="B669" s="2" t="s">
         <v>653</v>
@@ -21826,7 +21832,7 @@
     </row>
     <row r="670" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A670" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B670" s="2" t="s">
         <v>653</v>
@@ -21854,7 +21860,7 @@
     </row>
     <row r="671" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A671" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B671" s="2" t="s">
         <v>653</v>
@@ -21882,7 +21888,7 @@
     </row>
     <row r="672" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A672" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B672" s="2" t="s">
         <v>653</v>
@@ -21910,7 +21916,7 @@
     </row>
     <row r="673" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A673" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B673" s="2" t="s">
         <v>653</v>
@@ -21938,7 +21944,7 @@
     </row>
     <row r="674" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A674" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B674" s="2" t="s">
         <v>653</v>
@@ -21966,7 +21972,7 @@
     </row>
     <row r="675" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B675" s="2" t="s">
         <v>653</v>
@@ -21994,7 +22000,7 @@
     </row>
     <row r="676" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A676" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B676" s="2" t="s">
         <v>653</v>
@@ -22022,7 +22028,7 @@
     </row>
     <row r="677" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A677" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B677" s="2" t="s">
         <v>653</v>
@@ -22050,7 +22056,7 @@
     </row>
     <row r="678" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A678" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B678" s="2" t="s">
         <v>653</v>
@@ -22078,7 +22084,7 @@
     </row>
     <row r="679" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A679" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B679" s="2" t="s">
         <v>653</v>
@@ -22106,7 +22112,7 @@
     </row>
     <row r="680" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A680" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B680" s="2" t="s">
         <v>653</v>
@@ -22134,7 +22140,7 @@
     </row>
     <row r="681" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A681" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B681" s="2" t="s">
         <v>653</v>
@@ -22162,7 +22168,7 @@
     </row>
     <row r="682" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B682" s="2" t="s">
         <v>653</v>
@@ -22190,7 +22196,7 @@
     </row>
     <row r="683" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A683" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B683" s="2" t="s">
         <v>653</v>
@@ -22218,7 +22224,7 @@
     </row>
     <row r="684" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A684" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B684" s="2" t="s">
         <v>653</v>
@@ -22246,7 +22252,7 @@
     </row>
     <row r="685" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A685" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B685" s="2" t="s">
         <v>653</v>
@@ -22274,7 +22280,7 @@
     </row>
     <row r="686" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A686" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B686" s="2" t="s">
         <v>653</v>
@@ -22302,7 +22308,7 @@
     </row>
     <row r="687" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B687" s="2" t="s">
         <v>653</v>
@@ -22330,7 +22336,7 @@
     </row>
     <row r="688" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A688" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B688" s="2" t="s">
         <v>653</v>
@@ -22358,7 +22364,7 @@
     </row>
     <row r="689" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A689" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B689" s="2" t="s">
         <v>653</v>
@@ -22386,7 +22392,7 @@
     </row>
     <row r="690" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A690" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B690" s="2" t="s">
         <v>653</v>
@@ -22414,7 +22420,7 @@
     </row>
     <row r="691" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A691" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B691" s="2" t="s">
         <v>653</v>
@@ -22442,7 +22448,7 @@
     </row>
     <row r="692" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B692" s="2" t="s">
         <v>653</v>
@@ -22470,7 +22476,7 @@
     </row>
     <row r="693" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A693" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B693" s="2" t="s">
         <v>653</v>
@@ -22498,7 +22504,7 @@
     </row>
     <row r="694" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A694" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B694" s="2" t="s">
         <v>653</v>
@@ -22526,7 +22532,7 @@
     </row>
     <row r="695" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A695" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B695" s="2" t="s">
         <v>653</v>
@@ -22554,7 +22560,7 @@
     </row>
     <row r="696" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A696" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B696" s="2" t="s">
         <v>653</v>
@@ -22582,7 +22588,7 @@
     </row>
     <row r="697" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A697" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B697" s="2" t="s">
         <v>653</v>
@@ -22610,7 +22616,7 @@
     </row>
     <row r="698" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A698" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B698" s="2" t="s">
         <v>653</v>
@@ -22638,10 +22644,10 @@
     </row>
     <row r="699" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A699" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>702</v>
+        <v>653</v>
       </c>
       <c r="C699" s="2"/>
       <c r="D699" s="3" t="b">
@@ -22666,7 +22672,7 @@
     </row>
     <row r="700" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A700" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B700" s="2" t="s">
         <v>702</v>
@@ -22694,7 +22700,7 @@
     </row>
     <row r="701" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A701" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B701" s="2" t="s">
         <v>702</v>
@@ -22722,7 +22728,7 @@
     </row>
     <row r="702" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A702" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B702" s="2" t="s">
         <v>702</v>
@@ -22750,7 +22756,7 @@
     </row>
     <row r="703" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A703" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B703" s="2" t="s">
         <v>702</v>
@@ -22778,7 +22784,7 @@
     </row>
     <row r="704" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A704" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B704" s="2" t="s">
         <v>702</v>
@@ -22806,7 +22812,7 @@
     </row>
     <row r="705" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B705" s="2" t="s">
         <v>702</v>
@@ -22834,7 +22840,7 @@
     </row>
     <row r="706" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A706" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B706" s="2" t="s">
         <v>702</v>
@@ -22862,7 +22868,7 @@
     </row>
     <row r="707" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A707" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B707" s="2" t="s">
         <v>702</v>
@@ -22890,7 +22896,7 @@
     </row>
     <row r="708" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A708" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B708" s="2" t="s">
         <v>702</v>
@@ -22918,7 +22924,7 @@
     </row>
     <row r="709" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B709" s="2" t="s">
         <v>702</v>
@@ -22946,7 +22952,7 @@
     </row>
     <row r="710" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A710" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B710" s="2" t="s">
         <v>702</v>
@@ -22974,7 +22980,7 @@
     </row>
     <row r="711" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A711" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B711" s="2" t="s">
         <v>702</v>
@@ -23002,7 +23008,7 @@
     </row>
     <row r="712" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A712" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B712" s="2" t="s">
         <v>702</v>
@@ -23030,7 +23036,7 @@
     </row>
     <row r="713" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A713" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B713" s="2" t="s">
         <v>702</v>
@@ -23058,7 +23064,7 @@
     </row>
     <row r="714" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A714" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B714" s="2" t="s">
         <v>702</v>
@@ -23086,7 +23092,7 @@
     </row>
     <row r="715" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A715" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B715" s="2" t="s">
         <v>702</v>
@@ -23114,7 +23120,7 @@
     </row>
     <row r="716" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A716" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B716" s="2" t="s">
         <v>702</v>
@@ -23142,7 +23148,7 @@
     </row>
     <row r="717" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A717" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B717" s="2" t="s">
         <v>702</v>
@@ -23170,7 +23176,7 @@
     </row>
     <row r="718" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A718" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B718" s="2" t="s">
         <v>702</v>
@@ -23198,7 +23204,7 @@
     </row>
     <row r="719" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A719" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B719" s="2" t="s">
         <v>702</v>
@@ -23226,7 +23232,7 @@
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A720" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B720" s="2" t="s">
         <v>702</v>
@@ -23254,7 +23260,7 @@
     </row>
     <row r="721" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A721" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B721" s="2" t="s">
         <v>702</v>
@@ -23282,7 +23288,7 @@
     </row>
     <row r="722" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A722" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B722" s="2" t="s">
         <v>702</v>
@@ -23310,7 +23316,7 @@
     </row>
     <row r="723" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A723" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B723" s="2" t="s">
         <v>702</v>
@@ -23338,7 +23344,7 @@
     </row>
     <row r="724" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A724" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B724" s="2" t="s">
         <v>702</v>
@@ -23366,7 +23372,7 @@
     </row>
     <row r="725" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A725" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B725" s="2" t="s">
         <v>702</v>
@@ -23394,7 +23400,7 @@
     </row>
     <row r="726" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B726" s="2" t="s">
         <v>702</v>
@@ -23422,7 +23428,7 @@
     </row>
     <row r="727" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A727" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B727" s="2" t="s">
         <v>702</v>
@@ -23450,7 +23456,7 @@
     </row>
     <row r="728" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A728" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B728" s="2" t="s">
         <v>702</v>
@@ -23478,7 +23484,7 @@
     </row>
     <row r="729" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A729" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B729" s="2" t="s">
         <v>702</v>
@@ -23506,7 +23512,7 @@
     </row>
     <row r="730" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A730" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B730" s="2" t="s">
         <v>702</v>
@@ -23534,7 +23540,7 @@
     </row>
     <row r="731" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A731" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B731" s="2" t="s">
         <v>702</v>
@@ -23562,7 +23568,7 @@
     </row>
     <row r="732" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A732" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B732" s="2" t="s">
         <v>702</v>
@@ -23590,7 +23596,7 @@
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A733" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B733" s="2" t="s">
         <v>702</v>
@@ -23618,7 +23624,7 @@
     </row>
     <row r="734" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A734" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B734" s="2" t="s">
         <v>702</v>
@@ -23646,7 +23652,7 @@
     </row>
     <row r="735" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A735" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B735" s="2" t="s">
         <v>702</v>
@@ -23674,7 +23680,7 @@
     </row>
     <row r="736" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A736" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B736" s="2" t="s">
         <v>702</v>
@@ -23702,7 +23708,7 @@
     </row>
     <row r="737" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A737" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B737" s="2" t="s">
         <v>702</v>
@@ -23730,7 +23736,7 @@
     </row>
     <row r="738" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A738" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B738" s="2" t="s">
         <v>702</v>
@@ -23758,7 +23764,7 @@
     </row>
     <row r="739" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A739" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B739" s="2" t="s">
         <v>702</v>
@@ -23786,7 +23792,7 @@
     </row>
     <row r="740" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A740" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B740" s="2" t="s">
         <v>702</v>
@@ -23814,7 +23820,7 @@
     </row>
     <row r="741" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A741" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B741" s="2" t="s">
         <v>702</v>
@@ -23842,7 +23848,7 @@
     </row>
     <row r="742" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A742" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B742" s="2" t="s">
         <v>702</v>
@@ -23870,7 +23876,7 @@
     </row>
     <row r="743" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A743" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B743" s="2" t="s">
         <v>702</v>
@@ -23898,7 +23904,7 @@
     </row>
     <row r="744" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A744" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B744" s="2" t="s">
         <v>702</v>
@@ -23926,7 +23932,7 @@
     </row>
     <row r="745" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A745" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B745" s="2" t="s">
         <v>702</v>
@@ -23954,7 +23960,7 @@
     </row>
     <row r="746" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A746" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B746" s="2" t="s">
         <v>702</v>
@@ -23982,7 +23988,7 @@
     </row>
     <row r="747" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A747" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B747" s="2" t="s">
         <v>702</v>
@@ -24010,7 +24016,7 @@
     </row>
     <row r="748" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A748" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B748" s="2" t="s">
         <v>702</v>
@@ -24038,10 +24044,10 @@
     </row>
     <row r="749" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>654</v>
+        <v>751</v>
       </c>
       <c r="B749" s="2" t="s">
-        <v>752</v>
+        <v>702</v>
       </c>
       <c r="C749" s="2"/>
       <c r="D749" s="3" t="b">
@@ -24066,7 +24072,7 @@
     </row>
     <row r="750" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A750" s="2" t="s">
-        <v>753</v>
+        <v>654</v>
       </c>
       <c r="B750" s="2" t="s">
         <v>752</v>
@@ -24094,7 +24100,7 @@
     </row>
     <row r="751" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A751" s="2" t="s">
-        <v>212</v>
+        <v>753</v>
       </c>
       <c r="B751" s="2" t="s">
         <v>752</v>
@@ -24122,7 +24128,7 @@
     </row>
     <row r="752" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A752" s="2" t="s">
-        <v>754</v>
+        <v>212</v>
       </c>
       <c r="B752" s="2" t="s">
         <v>752</v>
@@ -24150,7 +24156,7 @@
     </row>
     <row r="753" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A753" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B753" s="2" t="s">
         <v>752</v>
@@ -24178,7 +24184,7 @@
     </row>
     <row r="754" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A754" s="2" t="s">
-        <v>218</v>
+        <v>755</v>
       </c>
       <c r="B754" s="2" t="s">
         <v>752</v>
@@ -24206,7 +24212,7 @@
     </row>
     <row r="755" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A755" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B755" s="2" t="s">
         <v>752</v>
@@ -24234,7 +24240,7 @@
     </row>
     <row r="756" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A756" s="2" t="s">
-        <v>662</v>
+        <v>220</v>
       </c>
       <c r="B756" s="2" t="s">
         <v>752</v>
@@ -24262,7 +24268,7 @@
     </row>
     <row r="757" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A757" s="2" t="s">
-        <v>756</v>
+        <v>662</v>
       </c>
       <c r="B757" s="2" t="s">
         <v>752</v>
@@ -24290,7 +24296,7 @@
     </row>
     <row r="758" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A758" s="2" t="s">
-        <v>20</v>
+        <v>756</v>
       </c>
       <c r="B758" s="2" t="s">
         <v>752</v>
@@ -24318,7 +24324,7 @@
     </row>
     <row r="759" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A759" s="2" t="s">
-        <v>757</v>
+        <v>20</v>
       </c>
       <c r="B759" s="2" t="s">
         <v>752</v>
@@ -24346,7 +24352,7 @@
     </row>
     <row r="760" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A760" s="2" t="s">
-        <v>330</v>
+        <v>757</v>
       </c>
       <c r="B760" s="2" t="s">
         <v>752</v>
@@ -24374,7 +24380,7 @@
     </row>
     <row r="761" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A761" s="2" t="s">
-        <v>758</v>
+        <v>330</v>
       </c>
       <c r="B761" s="2" t="s">
         <v>752</v>
@@ -24402,7 +24408,7 @@
     </row>
     <row r="762" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A762" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B762" s="2" t="s">
         <v>752</v>
@@ -24430,7 +24436,7 @@
     </row>
     <row r="763" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A763" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B763" s="2" t="s">
         <v>752</v>
@@ -24458,7 +24464,7 @@
     </row>
     <row r="764" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A764" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B764" s="2" t="s">
         <v>752</v>
@@ -24486,7 +24492,7 @@
     </row>
     <row r="765" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A765" s="2" t="s">
-        <v>23</v>
+        <v>761</v>
       </c>
       <c r="B765" s="2" t="s">
         <v>752</v>
@@ -24514,7 +24520,7 @@
     </row>
     <row r="766" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A766" s="2" t="s">
-        <v>762</v>
+        <v>23</v>
       </c>
       <c r="B766" s="2" t="s">
         <v>752</v>
@@ -24542,7 +24548,7 @@
     </row>
     <row r="767" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A767" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B767" s="2" t="s">
         <v>752</v>
@@ -24570,7 +24576,7 @@
     </row>
     <row r="768" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A768" s="2" t="s">
-        <v>24</v>
+        <v>763</v>
       </c>
       <c r="B768" s="2" t="s">
         <v>752</v>
@@ -24598,7 +24604,7 @@
     </row>
     <row r="769" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A769" s="2" t="s">
-        <v>764</v>
+        <v>24</v>
       </c>
       <c r="B769" s="2" t="s">
         <v>752</v>
@@ -24626,7 +24632,7 @@
     </row>
     <row r="770" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A770" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B770" s="2" t="s">
         <v>752</v>
@@ -24654,7 +24660,7 @@
     </row>
     <row r="771" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A771" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B771" s="2" t="s">
         <v>752</v>
@@ -24682,7 +24688,7 @@
     </row>
     <row r="772" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A772" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B772" s="2" t="s">
         <v>752</v>
@@ -24710,7 +24716,7 @@
     </row>
     <row r="773" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A773" s="2" t="s">
-        <v>237</v>
+        <v>767</v>
       </c>
       <c r="B773" s="2" t="s">
         <v>752</v>
@@ -24738,7 +24744,7 @@
     </row>
     <row r="774" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A774" s="2" t="s">
-        <v>768</v>
+        <v>237</v>
       </c>
       <c r="B774" s="2" t="s">
         <v>752</v>
@@ -24766,7 +24772,7 @@
     </row>
     <row r="775" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A775" s="2" t="s">
-        <v>29</v>
+        <v>768</v>
       </c>
       <c r="B775" s="2" t="s">
         <v>752</v>
@@ -24794,7 +24800,7 @@
     </row>
     <row r="776" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A776" s="2" t="s">
-        <v>632</v>
+        <v>29</v>
       </c>
       <c r="B776" s="2" t="s">
         <v>752</v>
@@ -24822,7 +24828,7 @@
     </row>
     <row r="777" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A777" s="2" t="s">
-        <v>769</v>
+        <v>632</v>
       </c>
       <c r="B777" s="2" t="s">
         <v>752</v>
@@ -24850,7 +24856,7 @@
     </row>
     <row r="778" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A778" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B778" s="2" t="s">
         <v>752</v>
@@ -24878,7 +24884,7 @@
     </row>
     <row r="779" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A779" s="2" t="s">
-        <v>347</v>
+        <v>770</v>
       </c>
       <c r="B779" s="2" t="s">
         <v>752</v>
@@ -24906,7 +24912,7 @@
     </row>
     <row r="780" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A780" s="2" t="s">
-        <v>771</v>
+        <v>347</v>
       </c>
       <c r="B780" s="2" t="s">
         <v>752</v>
@@ -24934,7 +24940,7 @@
     </row>
     <row r="781" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A781" s="2" t="s">
-        <v>486</v>
+        <v>771</v>
       </c>
       <c r="B781" s="2" t="s">
         <v>752</v>
@@ -24962,7 +24968,7 @@
     </row>
     <row r="782" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A782" s="2" t="s">
-        <v>32</v>
+        <v>486</v>
       </c>
       <c r="B782" s="2" t="s">
         <v>752</v>
@@ -24990,7 +24996,7 @@
     </row>
     <row r="783" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A783" s="2" t="s">
-        <v>772</v>
+        <v>32</v>
       </c>
       <c r="B783" s="2" t="s">
         <v>752</v>
@@ -25018,7 +25024,7 @@
     </row>
     <row r="784" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A784" s="2" t="s">
-        <v>34</v>
+        <v>772</v>
       </c>
       <c r="B784" s="2" t="s">
         <v>752</v>
@@ -25046,7 +25052,7 @@
     </row>
     <row r="785" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A785" s="2" t="s">
-        <v>773</v>
+        <v>34</v>
       </c>
       <c r="B785" s="2" t="s">
         <v>752</v>
@@ -25074,7 +25080,7 @@
     </row>
     <row r="786" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A786" s="2" t="s">
-        <v>36</v>
+        <v>773</v>
       </c>
       <c r="B786" s="2" t="s">
         <v>752</v>
@@ -25102,7 +25108,7 @@
     </row>
     <row r="787" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A787" s="2" t="s">
-        <v>774</v>
+        <v>36</v>
       </c>
       <c r="B787" s="2" t="s">
         <v>752</v>
@@ -25130,7 +25136,7 @@
     </row>
     <row r="788" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A788" s="2" t="s">
-        <v>37</v>
+        <v>774</v>
       </c>
       <c r="B788" s="2" t="s">
         <v>752</v>
@@ -25158,7 +25164,7 @@
     </row>
     <row r="789" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A789" s="2" t="s">
-        <v>775</v>
+        <v>37</v>
       </c>
       <c r="B789" s="2" t="s">
         <v>752</v>
@@ -25186,7 +25192,7 @@
     </row>
     <row r="790" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A790" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B790" s="2" t="s">
         <v>752</v>
@@ -25214,7 +25220,7 @@
     </row>
     <row r="791" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A791" s="2" t="s">
-        <v>39</v>
+        <v>776</v>
       </c>
       <c r="B791" s="2" t="s">
         <v>752</v>
@@ -25242,7 +25248,7 @@
     </row>
     <row r="792" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A792" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B792" s="2" t="s">
         <v>752</v>
@@ -25270,7 +25276,7 @@
     </row>
     <row r="793" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A793" s="2" t="s">
-        <v>645</v>
+        <v>40</v>
       </c>
       <c r="B793" s="2" t="s">
         <v>752</v>
@@ -25298,7 +25304,7 @@
     </row>
     <row r="794" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A794" s="2" t="s">
-        <v>777</v>
+        <v>645</v>
       </c>
       <c r="B794" s="2" t="s">
         <v>752</v>
@@ -25326,7 +25332,7 @@
     </row>
     <row r="795" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A795" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B795" s="2" t="s">
         <v>752</v>
@@ -25354,7 +25360,7 @@
     </row>
     <row r="796" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A796" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B796" s="2" t="s">
         <v>752</v>
@@ -25382,7 +25388,7 @@
     </row>
     <row r="797" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A797" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B797" s="2" t="s">
         <v>752</v>
@@ -25410,7 +25416,7 @@
     </row>
     <row r="798" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A798" s="2" t="s">
-        <v>44</v>
+        <v>780</v>
       </c>
       <c r="B798" s="2" t="s">
         <v>752</v>
@@ -25438,10 +25444,10 @@
     </row>
     <row r="799" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A799" s="2" t="s">
-        <v>781</v>
+        <v>44</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>782</v>
+        <v>752</v>
       </c>
       <c r="C799" s="2"/>
       <c r="D799" s="3" t="b">
@@ -25466,7 +25472,7 @@
     </row>
     <row r="800" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A800" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B800" s="2" t="s">
         <v>782</v>
@@ -25494,7 +25500,7 @@
     </row>
     <row r="801" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A801" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B801" s="2" t="s">
         <v>782</v>
@@ -25522,7 +25528,7 @@
     </row>
     <row r="802" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A802" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B802" s="2" t="s">
         <v>782</v>
@@ -25550,7 +25556,7 @@
     </row>
     <row r="803" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A803" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B803" s="2" t="s">
         <v>782</v>
@@ -25578,7 +25584,7 @@
     </row>
     <row r="804" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A804" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B804" s="2" t="s">
         <v>782</v>
@@ -25606,7 +25612,7 @@
     </row>
     <row r="805" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A805" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B805" s="2" t="s">
         <v>782</v>
@@ -25634,7 +25640,7 @@
     </row>
     <row r="806" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A806" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B806" s="2" t="s">
         <v>782</v>
@@ -25662,7 +25668,7 @@
     </row>
     <row r="807" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A807" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B807" s="2" t="s">
         <v>782</v>
@@ -25690,7 +25696,7 @@
     </row>
     <row r="808" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A808" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B808" s="2" t="s">
         <v>782</v>
@@ -25718,7 +25724,7 @@
     </row>
     <row r="809" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A809" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B809" s="2" t="s">
         <v>782</v>
@@ -25746,7 +25752,7 @@
     </row>
     <row r="810" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A810" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B810" s="2" t="s">
         <v>782</v>
@@ -25774,7 +25780,7 @@
     </row>
     <row r="811" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A811" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B811" s="2" t="s">
         <v>782</v>
@@ -25802,7 +25808,7 @@
     </row>
     <row r="812" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A812" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B812" s="2" t="s">
         <v>782</v>
@@ -25830,7 +25836,7 @@
     </row>
     <row r="813" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A813" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B813" s="2" t="s">
         <v>782</v>
@@ -25858,7 +25864,7 @@
     </row>
     <row r="814" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A814" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B814" s="2" t="s">
         <v>782</v>
@@ -25886,7 +25892,7 @@
     </row>
     <row r="815" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A815" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B815" s="2" t="s">
         <v>782</v>
@@ -25914,7 +25920,7 @@
     </row>
     <row r="816" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A816" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B816" s="2" t="s">
         <v>782</v>
@@ -25942,7 +25948,7 @@
     </row>
     <row r="817" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A817" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B817" s="2" t="s">
         <v>782</v>
@@ -25970,7 +25976,7 @@
     </row>
     <row r="818" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A818" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B818" s="2" t="s">
         <v>782</v>
@@ -25998,7 +26004,7 @@
     </row>
     <row r="819" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A819" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B819" s="2" t="s">
         <v>782</v>
@@ -26026,7 +26032,7 @@
     </row>
     <row r="820" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A820" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B820" s="2" t="s">
         <v>782</v>
@@ -26054,7 +26060,7 @@
     </row>
     <row r="821" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A821" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B821" s="2" t="s">
         <v>782</v>
@@ -26082,7 +26088,7 @@
     </row>
     <row r="822" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A822" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B822" s="2" t="s">
         <v>782</v>
@@ -26110,7 +26116,7 @@
     </row>
     <row r="823" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A823" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B823" s="2" t="s">
         <v>782</v>
@@ -26138,7 +26144,7 @@
     </row>
     <row r="824" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A824" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B824" s="2" t="s">
         <v>782</v>
@@ -26166,7 +26172,7 @@
     </row>
     <row r="825" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A825" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>782</v>
@@ -26194,7 +26200,7 @@
     </row>
     <row r="826" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A826" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B826" s="2" t="s">
         <v>782</v>
@@ -26222,7 +26228,7 @@
     </row>
     <row r="827" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A827" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B827" s="2" t="s">
         <v>782</v>
@@ -26250,7 +26256,7 @@
     </row>
     <row r="828" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A828" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B828" s="2" t="s">
         <v>782</v>
@@ -26278,7 +26284,7 @@
     </row>
     <row r="829" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A829" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B829" s="2" t="s">
         <v>782</v>
@@ -26306,7 +26312,7 @@
     </row>
     <row r="830" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A830" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B830" s="2" t="s">
         <v>782</v>
@@ -26334,7 +26340,7 @@
     </row>
     <row r="831" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A831" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B831" s="2" t="s">
         <v>782</v>
@@ -26362,7 +26368,7 @@
     </row>
     <row r="832" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A832" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B832" s="2" t="s">
         <v>782</v>
@@ -26390,7 +26396,7 @@
     </row>
     <row r="833" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A833" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B833" s="2" t="s">
         <v>782</v>
@@ -26418,7 +26424,7 @@
     </row>
     <row r="834" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A834" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B834" s="2" t="s">
         <v>782</v>
@@ -26446,7 +26452,7 @@
     </row>
     <row r="835" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A835" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B835" s="2" t="s">
         <v>782</v>
@@ -26474,7 +26480,7 @@
     </row>
     <row r="836" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A836" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B836" s="2" t="s">
         <v>782</v>
@@ -26502,7 +26508,7 @@
     </row>
     <row r="837" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A837" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B837" s="2" t="s">
         <v>782</v>
@@ -26530,7 +26536,7 @@
     </row>
     <row r="838" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A838" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B838" s="2" t="s">
         <v>782</v>
@@ -26558,7 +26564,7 @@
     </row>
     <row r="839" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A839" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B839" s="2" t="s">
         <v>782</v>
@@ -26586,7 +26592,7 @@
     </row>
     <row r="840" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A840" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B840" s="2" t="s">
         <v>782</v>
@@ -26614,7 +26620,7 @@
     </row>
     <row r="841" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A841" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B841" s="2" t="s">
         <v>782</v>
@@ -26642,7 +26648,7 @@
     </row>
     <row r="842" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A842" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B842" s="2" t="s">
         <v>782</v>
@@ -26670,7 +26676,7 @@
     </row>
     <row r="843" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A843" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B843" s="2" t="s">
         <v>782</v>
@@ -26698,7 +26704,7 @@
     </row>
     <row r="844" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A844" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B844" s="2" t="s">
         <v>782</v>
@@ -26726,10 +26732,10 @@
     </row>
     <row r="845" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A845" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>829</v>
+        <v>782</v>
       </c>
       <c r="C845" s="2"/>
       <c r="D845" s="3" t="b">
@@ -26754,7 +26760,7 @@
     </row>
     <row r="846" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A846" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B846" s="2" t="s">
         <v>829</v>
@@ -26782,7 +26788,7 @@
     </row>
     <row r="847" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A847" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B847" s="2" t="s">
         <v>829</v>
@@ -26810,7 +26816,7 @@
     </row>
     <row r="848" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A848" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B848" s="2" t="s">
         <v>829</v>
@@ -26838,7 +26844,7 @@
     </row>
     <row r="849" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A849" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B849" s="2" t="s">
         <v>829</v>
@@ -26866,7 +26872,7 @@
     </row>
     <row r="850" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A850" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B850" s="2" t="s">
         <v>829</v>
@@ -26894,7 +26900,7 @@
     </row>
     <row r="851" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A851" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B851" s="2" t="s">
         <v>829</v>
@@ -26922,7 +26928,7 @@
     </row>
     <row r="852" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A852" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B852" s="2" t="s">
         <v>829</v>
@@ -26950,7 +26956,7 @@
     </row>
     <row r="853" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A853" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B853" s="2" t="s">
         <v>829</v>
@@ -26978,7 +26984,7 @@
     </row>
     <row r="854" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A854" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B854" s="2" t="s">
         <v>829</v>
@@ -27006,7 +27012,7 @@
     </row>
     <row r="855" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A855" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B855" s="2" t="s">
         <v>829</v>
@@ -27034,7 +27040,7 @@
     </row>
     <row r="856" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A856" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B856" s="2" t="s">
         <v>829</v>
@@ -27062,7 +27068,7 @@
     </row>
     <row r="857" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A857" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B857" s="2" t="s">
         <v>829</v>
@@ -27090,7 +27096,7 @@
     </row>
     <row r="858" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A858" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B858" s="2" t="s">
         <v>829</v>
@@ -27118,7 +27124,7 @@
     </row>
     <row r="859" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A859" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B859" s="2" t="s">
         <v>829</v>
@@ -27146,7 +27152,7 @@
     </row>
     <row r="860" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A860" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B860" s="2" t="s">
         <v>829</v>
@@ -27174,7 +27180,7 @@
     </row>
     <row r="861" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A861" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B861" s="2" t="s">
         <v>829</v>
@@ -27202,7 +27208,7 @@
     </row>
     <row r="862" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A862" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B862" s="2" t="s">
         <v>829</v>
@@ -27230,7 +27236,7 @@
     </row>
     <row r="863" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A863" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B863" s="2" t="s">
         <v>829</v>
@@ -27258,7 +27264,7 @@
     </row>
     <row r="864" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A864" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B864" s="2" t="s">
         <v>829</v>
@@ -27286,7 +27292,7 @@
     </row>
     <row r="865" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A865" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B865" s="2" t="s">
         <v>829</v>
@@ -27314,7 +27320,7 @@
     </row>
     <row r="866" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A866" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B866" s="2" t="s">
         <v>829</v>
@@ -27342,7 +27348,7 @@
     </row>
     <row r="867" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A867" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B867" s="2" t="s">
         <v>829</v>
@@ -27370,7 +27376,7 @@
     </row>
     <row r="868" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A868" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B868" s="2" t="s">
         <v>829</v>
@@ -27398,7 +27404,7 @@
     </row>
     <row r="869" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A869" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B869" s="2" t="s">
         <v>829</v>
@@ -27426,7 +27432,7 @@
     </row>
     <row r="870" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A870" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B870" s="2" t="s">
         <v>829</v>
@@ -27454,7 +27460,7 @@
     </row>
     <row r="871" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A871" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B871" s="2" t="s">
         <v>829</v>
@@ -27482,7 +27488,7 @@
     </row>
     <row r="872" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A872" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B872" s="2" t="s">
         <v>829</v>
@@ -27510,7 +27516,7 @@
     </row>
     <row r="873" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A873" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B873" s="2" t="s">
         <v>829</v>
@@ -27538,7 +27544,7 @@
     </row>
     <row r="874" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A874" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B874" s="2" t="s">
         <v>829</v>
@@ -27566,7 +27572,7 @@
     </row>
     <row r="875" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A875" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B875" s="2" t="s">
         <v>829</v>
@@ -27594,7 +27600,7 @@
     </row>
     <row r="876" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A876" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B876" s="2" t="s">
         <v>829</v>
@@ -27622,7 +27628,7 @@
     </row>
     <row r="877" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A877" s="2" t="s">
-        <v>741</v>
+        <v>860</v>
       </c>
       <c r="B877" s="2" t="s">
         <v>829</v>
@@ -27650,7 +27656,7 @@
     </row>
     <row r="878" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A878" s="2" t="s">
-        <v>861</v>
+        <v>741</v>
       </c>
       <c r="B878" s="2" t="s">
         <v>829</v>
@@ -27678,7 +27684,7 @@
     </row>
     <row r="879" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A879" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B879" s="2" t="s">
         <v>829</v>
@@ -27706,7 +27712,7 @@
     </row>
     <row r="880" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A880" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B880" s="2" t="s">
         <v>829</v>
@@ -27734,7 +27740,7 @@
     </row>
     <row r="881" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A881" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B881" s="2" t="s">
         <v>829</v>
@@ -27762,7 +27768,7 @@
     </row>
     <row r="882" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A882" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B882" s="2" t="s">
         <v>829</v>
@@ -27790,7 +27796,7 @@
     </row>
     <row r="883" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A883" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B883" s="2" t="s">
         <v>829</v>
@@ -27818,7 +27824,7 @@
     </row>
     <row r="884" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A884" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B884" s="2" t="s">
         <v>829</v>
@@ -27846,7 +27852,7 @@
     </row>
     <row r="885" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A885" s="2" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B885" s="2" t="s">
         <v>829</v>
@@ -27874,7 +27880,7 @@
     </row>
     <row r="886" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A886" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B886" s="2" t="s">
         <v>829</v>
@@ -27902,7 +27908,7 @@
     </row>
     <row r="887" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A887" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B887" s="2" t="s">
         <v>829</v>
@@ -27930,7 +27936,7 @@
     </row>
     <row r="888" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A888" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B888" s="2" t="s">
         <v>829</v>
@@ -27958,7 +27964,7 @@
     </row>
     <row r="889" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A889" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B889" s="2" t="s">
         <v>829</v>
@@ -27986,7 +27992,7 @@
     </row>
     <row r="890" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A890" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B890" s="2" t="s">
         <v>829</v>
@@ -28014,7 +28020,7 @@
     </row>
     <row r="891" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A891" s="2" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B891" s="2" t="s">
         <v>829</v>
@@ -28042,7 +28048,7 @@
     </row>
     <row r="892" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A892" s="2" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B892" s="2" t="s">
         <v>829</v>
@@ -28070,7 +28076,7 @@
     </row>
     <row r="893" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A893" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B893" s="2" t="s">
         <v>829</v>
@@ -28093,6 +28099,34 @@
       </c>
       <c r="I893" s="2"/>
       <c r="J893" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="894" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A894" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B894" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="C894" s="2"/>
+      <c r="D894" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E894" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F894" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G894" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H894" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I894" s="2"/>
+      <c r="J894" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix indentation in elegant_app.py, add Excel data file, and update .gitignore to exclude debug artifacts
</commit_message>
<xml_diff>
--- a/comprehensive_grocery_certifications.xlsx
+++ b/comprehensive_grocery_certifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StardogChampion\tbl-dev-workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StardogChampion\TBL-Grocery-Scanner---DEVELOPMENT-VERSION-Active-development--main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2EDDCBD-9074-4CDD-B1DF-C9BD7E9DA9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CC347-1270-4068-A42C-C2C76D4F58D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -3217,7 +3217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J941"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A472" sqref="A472"/>
     </sheetView>
@@ -29599,7 +29599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -30185,7 +30185,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <f ca="1">NOW()</f>
-        <v>46047.478419328705</v>
+        <v>46068.380347916667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Baby Ruth in Excel sheet
</commit_message>
<xml_diff>
--- a/comprehensive_grocery_certifications.xlsx
+++ b/comprehensive_grocery_certifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StardogChampion\TBL-Grocery-Scanner---DEVELOPMENT-VERSION-Active-development--main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FE0467-113C-4400-B03C-1EC4B9F888A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A66EEEF7-48CC-4A5A-9F74-D0A5B2A6ACA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="949">
   <si>
     <t>Product_Brand</t>
   </si>
@@ -3278,8 +3278,8 @@
   <dimension ref="A1:K947"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A687" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A698" sqref="A698"/>
+      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A287" sqref="A287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10686,24 +10686,26 @@
       </c>
       <c r="C255" s="2"/>
       <c r="D255" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E255" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F255" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G255" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H255" s="7"/>
+      <c r="H255" s="7" t="s">
+        <v>932</v>
+      </c>
       <c r="I255" s="3" t="b">
         <v>0</v>
       </c>
       <c r="J255" s="2"/>
       <c r="K255" s="2" t="s">
-        <v>11</v>
+        <v>879</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.3">
@@ -30888,17 +30890,17 @@
       <c r="C3">
         <f>COUNTIFS(Certifications!$B$2:$B$5006, Statistics!$A3,
           Certifications!$D$2:$D$5006, TRUE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f>COUNTIFS(Certifications!$B$2:$B$5006, Statistics!$A3,
           Certifications!$E$2:$E$5006, TRUE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <f>COUNTIFS(Certifications!$B$2:$B$5006, Statistics!$A3,
           Certifications!$F$2:$F$5006, TRUE)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <f>COUNTIFS(Certifications!$B$2:$B$5006, Statistics!$A3,
@@ -31405,7 +31407,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <f ca="1">NOW()</f>
-        <v>46073.679235069445</v>
+        <v>46073.695904282409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited nescafe in Excel sheet
</commit_message>
<xml_diff>
--- a/comprehensive_grocery_certifications.xlsx
+++ b/comprehensive_grocery_certifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StardogChampion\TBL-Grocery-Scanner---DEVELOPMENT-VERSION-Active-development--main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01CD5CE0-22BA-4ABE-9364-CCBDAFFABAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58465B4D-8C3D-4964-9326-5758CED4E6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="951">
   <si>
     <t>Product_Brand</t>
   </si>
@@ -2871,6 +2871,9 @@
   </si>
   <si>
     <t>Pure Life</t>
+  </si>
+  <si>
+    <t>iced coffee</t>
   </si>
 </sst>
 </file>
@@ -3281,8 +3284,8 @@
   <dimension ref="A1:K946"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
+      <pane ySplit="1" topLeftCell="A443" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A456" sqref="A456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6752,7 +6755,9 @@
       <c r="G119" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H119" s="7"/>
+      <c r="H119" s="7" t="s">
+        <v>950</v>
+      </c>
       <c r="I119" s="3" t="b">
         <v>0</v>
       </c>
@@ -31385,7 +31390,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <f ca="1">NOW()</f>
-        <v>46074.342800925922</v>
+        <v>46074.347226157406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>